<commit_message>
manque que les exo
</commit_message>
<xml_diff>
--- a/Physiopathologie/Excel/renale.xlsx
+++ b/Physiopathologie/Excel/renale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moito\Desktop\Sérieux\Projet\Site web\Physiopathologie\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8851E230-D510-49A1-830A-2012CE41D8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1AC6A8-8E79-42CD-AC20-915B731218AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0C1EC4D3-5916-499C-9244-5ABC4AEA4E79}"/>
   </bookViews>
@@ -782,9 +782,6 @@
     <t xml:space="preserve">Q31. Concernant les protéinuries, caractériser par Vrai ou Faux chacune des propositions suivantes.  </t>
   </si>
   <si>
-    <t xml:space="preserve"> La protéinurie physiologique &lt; 150 mg/24h comprend + 50% de protéines de bas poids moléculaire dont l'albumine et 450% de protéines tubulaires de Tamm-Horsfall.   </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Si le profil électrophorétique des protéines urinaires est identique à celui de l'électrophorèse des protéines plasmatiques, une protéinurie tubulaire non sélective doit être suspectée.    </t>
   </si>
   <si>
@@ -1524,6 +1521,9 @@
   </si>
   <si>
     <t>c'est 82%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La protéinurie physiologique &lt; 150 mg/24h comprend +ou- 50% de protéines de bas poids moléculaire dont l'albumine et +ou- 50% de protéines tubulaires de Tamm-Horsfall.   </t>
   </si>
 </sst>
 </file>
@@ -1905,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4434D7D-6CBE-4AEC-87F6-B0BB4C058CB9}">
   <dimension ref="A1:F308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D204" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E213" sqref="E213"/>
+    <sheetView tabSelected="1" topLeftCell="C291" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C298" sqref="C298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -2043,7 +2043,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -2083,7 +2083,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -2103,13 +2103,13 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
         <v>263</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>264</v>
       </c>
       <c r="F10" t="s">
         <v>6</v>
@@ -2209,7 +2209,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
@@ -2229,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
@@ -2343,13 +2343,13 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
+        <v>267</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>268</v>
-      </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>269</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
@@ -2409,7 +2409,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -2449,7 +2449,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F27" t="s">
         <v>6</v>
@@ -2489,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
@@ -2589,7 +2589,7 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F34" t="s">
         <v>6</v>
@@ -2663,13 +2663,13 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
+        <v>273</v>
+      </c>
+      <c r="D38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
         <v>274</v>
-      </c>
-      <c r="D38" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" t="s">
-        <v>275</v>
       </c>
       <c r="F38" t="s">
         <v>6</v>
@@ -2689,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F39" t="s">
         <v>6</v>
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F42" t="s">
         <v>6</v>
@@ -2763,7 +2763,7 @@
         <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -2789,7 +2789,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F44" t="s">
         <v>6</v>
@@ -2803,7 +2803,7 @@
         <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
@@ -2849,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F47" t="s">
         <v>6</v>
@@ -2889,7 +2889,7 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F49" t="s">
         <v>6</v>
@@ -2969,7 +2969,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F53" t="s">
         <v>6</v>
@@ -2983,7 +2983,7 @@
         <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -3009,7 +3009,7 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -3023,7 +3023,7 @@
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
@@ -3049,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F57" t="s">
         <v>6</v>
@@ -3069,7 +3069,7 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F58" t="s">
         <v>6</v>
@@ -3089,7 +3089,7 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F59" t="s">
         <v>6</v>
@@ -3103,7 +3103,7 @@
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
@@ -3169,7 +3169,7 @@
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F63" t="s">
         <v>6</v>
@@ -3189,7 +3189,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F64" t="s">
         <v>6</v>
@@ -3203,7 +3203,7 @@
         <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
@@ -3229,7 +3229,7 @@
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F66" t="s">
         <v>6</v>
@@ -3249,7 +3249,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F67" t="s">
         <v>6</v>
@@ -3269,7 +3269,7 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F68" t="s">
         <v>6</v>
@@ -3309,7 +3309,7 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F70" t="s">
         <v>6</v>
@@ -3329,7 +3329,7 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F71" t="s">
         <v>6</v>
@@ -3363,7 +3363,7 @@
         <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D73" t="b">
         <v>1</v>
@@ -3409,7 +3409,7 @@
         <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F75" t="s">
         <v>6</v>
@@ -3489,7 +3489,7 @@
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F79" t="s">
         <v>6</v>
@@ -3500,10 +3500,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C80" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D80" t="b">
         <v>1</v>
@@ -3549,7 +3549,7 @@
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F82" t="s">
         <v>6</v>
@@ -3569,7 +3569,7 @@
         <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F83" t="s">
         <v>6</v>
@@ -3609,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F85" t="s">
         <v>6</v>
@@ -3623,7 +3623,7 @@
         <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
@@ -3689,7 +3689,7 @@
         <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F89" t="s">
         <v>6</v>
@@ -3783,7 +3783,7 @@
         <v>6</v>
       </c>
       <c r="C94" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D94" t="b">
         <v>1</v>
@@ -3803,7 +3803,7 @@
         <v>6</v>
       </c>
       <c r="C95" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D95" t="b">
         <v>1</v>
@@ -3829,7 +3829,7 @@
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F96" t="s">
         <v>6</v>
@@ -3843,7 +3843,7 @@
         <v>6</v>
       </c>
       <c r="C97" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D97" t="b">
         <v>1</v>
@@ -3869,7 +3869,7 @@
         <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F98" t="s">
         <v>6</v>
@@ -3883,13 +3883,13 @@
         <v>6</v>
       </c>
       <c r="C99" t="s">
+        <v>312</v>
+      </c>
+      <c r="D99" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" t="s">
         <v>313</v>
-      </c>
-      <c r="D99" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" t="s">
-        <v>314</v>
       </c>
       <c r="F99" t="s">
         <v>6</v>
@@ -3903,7 +3903,7 @@
         <v>6</v>
       </c>
       <c r="C100" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D100" t="b">
         <v>1</v>
@@ -3929,7 +3929,7 @@
         <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F101" t="s">
         <v>6</v>
@@ -3943,7 +3943,7 @@
         <v>6</v>
       </c>
       <c r="C102" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D102" t="b">
         <v>1</v>
@@ -3963,13 +3963,13 @@
         <v>6</v>
       </c>
       <c r="C103" t="s">
+        <v>317</v>
+      </c>
+      <c r="D103" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" t="s">
         <v>318</v>
-      </c>
-      <c r="D103" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" t="s">
-        <v>319</v>
       </c>
       <c r="F103" t="s">
         <v>6</v>
@@ -3983,13 +3983,13 @@
         <v>6</v>
       </c>
       <c r="C104" t="s">
+        <v>319</v>
+      </c>
+      <c r="D104" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" t="s">
         <v>320</v>
-      </c>
-      <c r="D104" t="b">
-        <v>0</v>
-      </c>
-      <c r="E104" t="s">
-        <v>321</v>
       </c>
       <c r="F104" t="s">
         <v>6</v>
@@ -4023,13 +4023,13 @@
         <v>6</v>
       </c>
       <c r="C106" t="s">
+        <v>321</v>
+      </c>
+      <c r="D106" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" t="s">
         <v>322</v>
-      </c>
-      <c r="D106" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" t="s">
-        <v>323</v>
       </c>
       <c r="F106" t="s">
         <v>6</v>
@@ -4063,7 +4063,7 @@
         <v>6</v>
       </c>
       <c r="C108" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D108" t="b">
         <v>1</v>
@@ -4109,7 +4109,7 @@
         <v>0</v>
       </c>
       <c r="E110" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F110" t="s">
         <v>6</v>
@@ -4123,7 +4123,7 @@
         <v>6</v>
       </c>
       <c r="C111" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D111" t="b">
         <v>1</v>
@@ -4183,7 +4183,7 @@
         <v>6</v>
       </c>
       <c r="C114" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D114" t="b">
         <v>1</v>
@@ -4203,13 +4203,13 @@
         <v>6</v>
       </c>
       <c r="C115" t="s">
+        <v>327</v>
+      </c>
+      <c r="D115" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" t="s">
         <v>328</v>
-      </c>
-      <c r="D115" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" t="s">
-        <v>329</v>
       </c>
       <c r="F115" t="s">
         <v>6</v>
@@ -4223,7 +4223,7 @@
         <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D116" t="b">
         <v>0</v>
@@ -4283,7 +4283,7 @@
         <v>6</v>
       </c>
       <c r="C119" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D119" t="b">
         <v>1</v>
@@ -4303,13 +4303,13 @@
         <v>6</v>
       </c>
       <c r="C120" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D120" t="b">
         <v>0</v>
       </c>
       <c r="E120" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F120" t="s">
         <v>6</v>
@@ -4323,13 +4323,13 @@
         <v>6</v>
       </c>
       <c r="C121" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D121" t="b">
         <v>0</v>
       </c>
       <c r="E121" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F121" t="s">
         <v>6</v>
@@ -4363,7 +4363,7 @@
         <v>6</v>
       </c>
       <c r="C123" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D123" t="b">
         <v>1</v>
@@ -4383,7 +4383,7 @@
         <v>6</v>
       </c>
       <c r="C124" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D124" t="b">
         <v>1</v>
@@ -4409,7 +4409,7 @@
         <v>0</v>
       </c>
       <c r="E125" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F125" t="s">
         <v>6</v>
@@ -4429,7 +4429,7 @@
         <v>0</v>
       </c>
       <c r="E126" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F126" t="s">
         <v>6</v>
@@ -4449,7 +4449,7 @@
         <v>0</v>
       </c>
       <c r="E127" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F127" t="s">
         <v>6</v>
@@ -4489,7 +4489,7 @@
         <v>0</v>
       </c>
       <c r="E129" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F129" t="s">
         <v>6</v>
@@ -4509,7 +4509,7 @@
         <v>1</v>
       </c>
       <c r="E130" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F130" t="s">
         <v>6</v>
@@ -4523,7 +4523,7 @@
         <v>6</v>
       </c>
       <c r="C131" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D131" t="b">
         <v>1</v>
@@ -4563,7 +4563,7 @@
         <v>6</v>
       </c>
       <c r="C133" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D133" t="b">
         <v>1</v>
@@ -4583,13 +4583,13 @@
         <v>6</v>
       </c>
       <c r="C134" t="s">
+        <v>344</v>
+      </c>
+      <c r="D134" t="b">
+        <v>0</v>
+      </c>
+      <c r="E134" t="s">
         <v>345</v>
-      </c>
-      <c r="D134" t="b">
-        <v>0</v>
-      </c>
-      <c r="E134" t="s">
-        <v>346</v>
       </c>
       <c r="F134" t="s">
         <v>6</v>
@@ -4609,7 +4609,7 @@
         <v>0</v>
       </c>
       <c r="E135" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F135" t="s">
         <v>6</v>
@@ -4629,7 +4629,7 @@
         <v>0</v>
       </c>
       <c r="E136" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F136" t="s">
         <v>6</v>
@@ -4663,7 +4663,7 @@
         <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D138" t="b">
         <v>1</v>
@@ -4683,7 +4683,7 @@
         <v>6</v>
       </c>
       <c r="C139" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D139" t="b">
         <v>1</v>
@@ -4703,13 +4703,13 @@
         <v>6</v>
       </c>
       <c r="C140" t="s">
+        <v>350</v>
+      </c>
+      <c r="D140" t="b">
+        <v>0</v>
+      </c>
+      <c r="E140" t="s">
         <v>351</v>
-      </c>
-      <c r="D140" t="b">
-        <v>0</v>
-      </c>
-      <c r="E140" t="s">
-        <v>352</v>
       </c>
       <c r="F140" t="s">
         <v>6</v>
@@ -4723,7 +4723,7 @@
         <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D141" t="b">
         <v>1</v>
@@ -4743,7 +4743,7 @@
         <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D142" t="b">
         <v>1</v>
@@ -4763,13 +4763,13 @@
         <v>6</v>
       </c>
       <c r="C143" t="s">
+        <v>354</v>
+      </c>
+      <c r="D143" t="b">
+        <v>1</v>
+      </c>
+      <c r="E143" t="s">
         <v>355</v>
-      </c>
-      <c r="D143" t="b">
-        <v>1</v>
-      </c>
-      <c r="E143" t="s">
-        <v>356</v>
       </c>
       <c r="F143" t="s">
         <v>6</v>
@@ -4783,7 +4783,7 @@
         <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D144" t="b">
         <v>1</v>
@@ -4829,7 +4829,7 @@
         <v>0</v>
       </c>
       <c r="E146" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F146" t="s">
         <v>6</v>
@@ -4849,7 +4849,7 @@
         <v>0</v>
       </c>
       <c r="E147" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F147" t="s">
         <v>6</v>
@@ -4889,7 +4889,7 @@
         <v>0</v>
       </c>
       <c r="E149" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F149" t="s">
         <v>6</v>
@@ -4929,7 +4929,7 @@
         <v>0</v>
       </c>
       <c r="E151" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F151" t="s">
         <v>6</v>
@@ -4943,13 +4943,13 @@
         <v>6</v>
       </c>
       <c r="C152" t="s">
+        <v>360</v>
+      </c>
+      <c r="D152" t="b">
+        <v>0</v>
+      </c>
+      <c r="E152" t="s">
         <v>361</v>
-      </c>
-      <c r="D152" t="b">
-        <v>0</v>
-      </c>
-      <c r="E152" t="s">
-        <v>362</v>
       </c>
       <c r="F152" t="s">
         <v>6</v>
@@ -4969,7 +4969,7 @@
         <v>0</v>
       </c>
       <c r="E153" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F153" t="s">
         <v>6</v>
@@ -5023,7 +5023,7 @@
         <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D156" t="b">
         <v>1</v>
@@ -5103,13 +5103,13 @@
         <v>120</v>
       </c>
       <c r="C160" t="s">
+        <v>364</v>
+      </c>
+      <c r="D160" t="b">
+        <v>0</v>
+      </c>
+      <c r="E160" t="s">
         <v>365</v>
-      </c>
-      <c r="D160" t="b">
-        <v>0</v>
-      </c>
-      <c r="E160" t="s">
-        <v>366</v>
       </c>
       <c r="F160" t="s">
         <v>6</v>
@@ -5123,13 +5123,13 @@
         <v>120</v>
       </c>
       <c r="C161" t="s">
+        <v>366</v>
+      </c>
+      <c r="D161" t="b">
+        <v>0</v>
+      </c>
+      <c r="E161" t="s">
         <v>367</v>
-      </c>
-      <c r="D161" t="b">
-        <v>0</v>
-      </c>
-      <c r="E161" t="s">
-        <v>368</v>
       </c>
       <c r="F161" t="s">
         <v>6</v>
@@ -5149,7 +5149,7 @@
         <v>0</v>
       </c>
       <c r="E162" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F162" t="s">
         <v>6</v>
@@ -5163,7 +5163,7 @@
         <v>122</v>
       </c>
       <c r="C163" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D163" t="b">
         <v>1</v>
@@ -5189,7 +5189,7 @@
         <v>0</v>
       </c>
       <c r="E164" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F164" t="s">
         <v>6</v>
@@ -5223,7 +5223,7 @@
         <v>125</v>
       </c>
       <c r="C166" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D166" t="b">
         <v>1</v>
@@ -5289,7 +5289,7 @@
         <v>1</v>
       </c>
       <c r="E169" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F169" t="s">
         <v>6</v>
@@ -5323,13 +5323,13 @@
         <v>132</v>
       </c>
       <c r="C171" t="s">
+        <v>373</v>
+      </c>
+      <c r="D171" t="b">
+        <v>0</v>
+      </c>
+      <c r="E171" t="s">
         <v>374</v>
-      </c>
-      <c r="D171" t="b">
-        <v>0</v>
-      </c>
-      <c r="E171" t="s">
-        <v>375</v>
       </c>
       <c r="F171" t="s">
         <v>6</v>
@@ -5343,7 +5343,7 @@
         <v>132</v>
       </c>
       <c r="C172" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D172" t="b">
         <v>1</v>
@@ -5363,13 +5363,13 @@
         <v>132</v>
       </c>
       <c r="C173" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D173" t="b">
         <v>0</v>
       </c>
       <c r="E173" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F173" t="s">
         <v>6</v>
@@ -5383,7 +5383,7 @@
         <v>133</v>
       </c>
       <c r="C174" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D174" t="b">
         <v>1</v>
@@ -5403,7 +5403,7 @@
         <v>133</v>
       </c>
       <c r="C175" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D175" t="b">
         <v>1</v>
@@ -5469,7 +5469,7 @@
         <v>0</v>
       </c>
       <c r="E178" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F178" t="s">
         <v>6</v>
@@ -5503,13 +5503,13 @@
         <v>139</v>
       </c>
       <c r="C180" t="s">
+        <v>381</v>
+      </c>
+      <c r="D180" t="b">
+        <v>0</v>
+      </c>
+      <c r="E180" t="s">
         <v>382</v>
-      </c>
-      <c r="D180" t="b">
-        <v>0</v>
-      </c>
-      <c r="E180" t="s">
-        <v>383</v>
       </c>
       <c r="F180" t="s">
         <v>6</v>
@@ -5523,13 +5523,13 @@
         <v>139</v>
       </c>
       <c r="C181" t="s">
+        <v>383</v>
+      </c>
+      <c r="D181" t="b">
+        <v>0</v>
+      </c>
+      <c r="E181" t="s">
         <v>384</v>
-      </c>
-      <c r="D181" t="b">
-        <v>0</v>
-      </c>
-      <c r="E181" t="s">
-        <v>385</v>
       </c>
       <c r="F181" t="s">
         <v>6</v>
@@ -5543,13 +5543,13 @@
         <v>139</v>
       </c>
       <c r="C182" t="s">
+        <v>385</v>
+      </c>
+      <c r="D182" t="b">
+        <v>0</v>
+      </c>
+      <c r="E182" t="s">
         <v>386</v>
-      </c>
-      <c r="D182" t="b">
-        <v>0</v>
-      </c>
-      <c r="E182" t="s">
-        <v>387</v>
       </c>
       <c r="F182" t="s">
         <v>6</v>
@@ -5569,7 +5569,7 @@
         <v>0</v>
       </c>
       <c r="E183" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F183" t="s">
         <v>6</v>
@@ -5583,7 +5583,7 @@
         <v>140</v>
       </c>
       <c r="C184" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D184" t="b">
         <v>1</v>
@@ -5603,7 +5603,7 @@
         <v>140</v>
       </c>
       <c r="C185" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D185" t="b">
         <v>1</v>
@@ -5623,7 +5623,7 @@
         <v>142</v>
       </c>
       <c r="C186" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D186" t="b">
         <v>1</v>
@@ -5649,7 +5649,7 @@
         <v>0</v>
       </c>
       <c r="E187" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F187" t="s">
         <v>6</v>
@@ -5669,7 +5669,7 @@
         <v>0</v>
       </c>
       <c r="E188" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F188" t="s">
         <v>6</v>
@@ -5683,13 +5683,13 @@
         <v>145</v>
       </c>
       <c r="C189" t="s">
+        <v>393</v>
+      </c>
+      <c r="D189" t="b">
+        <v>0</v>
+      </c>
+      <c r="E189" t="s">
         <v>394</v>
-      </c>
-      <c r="D189" t="b">
-        <v>0</v>
-      </c>
-      <c r="E189" t="s">
-        <v>395</v>
       </c>
       <c r="F189" t="s">
         <v>6</v>
@@ -5709,7 +5709,7 @@
         <v>0</v>
       </c>
       <c r="E190" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F190" t="s">
         <v>6</v>
@@ -5723,13 +5723,13 @@
         <v>145</v>
       </c>
       <c r="C191" t="s">
+        <v>396</v>
+      </c>
+      <c r="D191" t="b">
+        <v>0</v>
+      </c>
+      <c r="E191" t="s">
         <v>397</v>
-      </c>
-      <c r="D191" t="b">
-        <v>0</v>
-      </c>
-      <c r="E191" t="s">
-        <v>398</v>
       </c>
       <c r="F191" t="s">
         <v>6</v>
@@ -5763,13 +5763,13 @@
         <v>147</v>
       </c>
       <c r="C193" t="s">
+        <v>398</v>
+      </c>
+      <c r="D193" t="b">
+        <v>0</v>
+      </c>
+      <c r="E193" t="s">
         <v>399</v>
-      </c>
-      <c r="D193" t="b">
-        <v>0</v>
-      </c>
-      <c r="E193" t="s">
-        <v>400</v>
       </c>
       <c r="F193" t="s">
         <v>6</v>
@@ -5803,13 +5803,13 @@
         <v>150</v>
       </c>
       <c r="C195" t="s">
+        <v>400</v>
+      </c>
+      <c r="D195" t="b">
+        <v>0</v>
+      </c>
+      <c r="E195" t="s">
         <v>401</v>
-      </c>
-      <c r="D195" t="b">
-        <v>0</v>
-      </c>
-      <c r="E195" t="s">
-        <v>402</v>
       </c>
       <c r="F195" t="s">
         <v>6</v>
@@ -5843,7 +5843,7 @@
         <v>150</v>
       </c>
       <c r="C197" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D197" t="b">
         <v>1</v>
@@ -5869,7 +5869,7 @@
         <v>0</v>
       </c>
       <c r="E198" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F198" t="s">
         <v>6</v>
@@ -5929,7 +5929,7 @@
         <v>1</v>
       </c>
       <c r="E201" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F201" t="s">
         <v>6</v>
@@ -5943,7 +5943,7 @@
         <v>156</v>
       </c>
       <c r="C202" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D202" t="b">
         <v>1</v>
@@ -5969,7 +5969,7 @@
         <v>0</v>
       </c>
       <c r="E203" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F203" t="s">
         <v>6</v>
@@ -5983,13 +5983,13 @@
         <v>159</v>
       </c>
       <c r="C204" t="s">
+        <v>407</v>
+      </c>
+      <c r="D204" t="b">
+        <v>0</v>
+      </c>
+      <c r="E204" t="s">
         <v>408</v>
-      </c>
-      <c r="D204" t="b">
-        <v>0</v>
-      </c>
-      <c r="E204" t="s">
-        <v>409</v>
       </c>
       <c r="F204" t="s">
         <v>6</v>
@@ -6003,13 +6003,13 @@
         <v>159</v>
       </c>
       <c r="C205" t="s">
+        <v>409</v>
+      </c>
+      <c r="D205" t="b">
+        <v>0</v>
+      </c>
+      <c r="E205" t="s">
         <v>410</v>
-      </c>
-      <c r="D205" t="b">
-        <v>0</v>
-      </c>
-      <c r="E205" t="s">
-        <v>411</v>
       </c>
       <c r="F205" t="s">
         <v>6</v>
@@ -6023,13 +6023,13 @@
         <v>159</v>
       </c>
       <c r="C206" t="s">
+        <v>411</v>
+      </c>
+      <c r="D206" t="b">
+        <v>1</v>
+      </c>
+      <c r="E206" t="s">
         <v>412</v>
-      </c>
-      <c r="D206" t="b">
-        <v>1</v>
-      </c>
-      <c r="E206" t="s">
-        <v>413</v>
       </c>
       <c r="F206" t="s">
         <v>6</v>
@@ -6049,7 +6049,7 @@
         <v>1</v>
       </c>
       <c r="E207" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F207" t="s">
         <v>6</v>
@@ -6063,13 +6063,13 @@
         <v>160</v>
       </c>
       <c r="C208" t="s">
+        <v>414</v>
+      </c>
+      <c r="D208" t="b">
+        <v>0</v>
+      </c>
+      <c r="E208" t="s">
         <v>415</v>
-      </c>
-      <c r="D208" t="b">
-        <v>0</v>
-      </c>
-      <c r="E208" t="s">
-        <v>416</v>
       </c>
       <c r="F208" t="s">
         <v>6</v>
@@ -6089,7 +6089,7 @@
         <v>0</v>
       </c>
       <c r="E209" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F209" t="s">
         <v>6</v>
@@ -6103,13 +6103,13 @@
         <v>163</v>
       </c>
       <c r="C210" t="s">
+        <v>417</v>
+      </c>
+      <c r="D210" t="b">
+        <v>1</v>
+      </c>
+      <c r="E210" t="s">
         <v>418</v>
-      </c>
-      <c r="D210" t="b">
-        <v>1</v>
-      </c>
-      <c r="E210" t="s">
-        <v>419</v>
       </c>
       <c r="F210" t="s">
         <v>6</v>
@@ -6149,7 +6149,7 @@
         <v>0</v>
       </c>
       <c r="E212" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F212" t="s">
         <v>6</v>
@@ -6183,7 +6183,7 @@
         <v>166</v>
       </c>
       <c r="C214" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D214" t="b">
         <v>1</v>
@@ -6223,7 +6223,7 @@
         <v>169</v>
       </c>
       <c r="C216" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D216" t="b">
         <v>1</v>
@@ -6263,13 +6263,13 @@
         <v>169</v>
       </c>
       <c r="C218" t="s">
+        <v>421</v>
+      </c>
+      <c r="D218" t="b">
+        <v>0</v>
+      </c>
+      <c r="E218" t="s">
         <v>422</v>
-      </c>
-      <c r="D218" t="b">
-        <v>0</v>
-      </c>
-      <c r="E218" t="s">
-        <v>423</v>
       </c>
       <c r="F218" t="s">
         <v>6</v>
@@ -6289,7 +6289,7 @@
         <v>0</v>
       </c>
       <c r="E219" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F219" t="s">
         <v>6</v>
@@ -6309,7 +6309,7 @@
         <v>0</v>
       </c>
       <c r="E220" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F220" t="s">
         <v>6</v>
@@ -6329,7 +6329,7 @@
         <v>0</v>
       </c>
       <c r="E221" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F221" t="s">
         <v>6</v>
@@ -6343,7 +6343,7 @@
         <v>175</v>
       </c>
       <c r="C222" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D222" t="b">
         <v>1</v>
@@ -6369,7 +6369,7 @@
         <v>0</v>
       </c>
       <c r="E223" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F223" t="s">
         <v>6</v>
@@ -6389,7 +6389,7 @@
         <v>0</v>
       </c>
       <c r="E224" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F224" t="s">
         <v>6</v>
@@ -6423,13 +6423,13 @@
         <v>178</v>
       </c>
       <c r="C226" t="s">
+        <v>429</v>
+      </c>
+      <c r="D226" t="b">
+        <v>1</v>
+      </c>
+      <c r="E226" t="s">
         <v>430</v>
-      </c>
-      <c r="D226" t="b">
-        <v>1</v>
-      </c>
-      <c r="E226" t="s">
-        <v>431</v>
       </c>
       <c r="F226" t="s">
         <v>6</v>
@@ -6469,7 +6469,7 @@
         <v>0</v>
       </c>
       <c r="E228" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F228" t="s">
         <v>6</v>
@@ -6483,7 +6483,7 @@
         <v>180</v>
       </c>
       <c r="C229" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D229" t="b">
         <v>1</v>
@@ -6503,7 +6503,7 @@
         <v>183</v>
       </c>
       <c r="C230" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D230" t="b">
         <v>1</v>
@@ -6529,7 +6529,7 @@
         <v>0</v>
       </c>
       <c r="E231" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F231" t="s">
         <v>6</v>
@@ -6549,7 +6549,7 @@
         <v>1</v>
       </c>
       <c r="E232" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F232" t="s">
         <v>6</v>
@@ -6563,7 +6563,7 @@
         <v>186</v>
       </c>
       <c r="C233" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D233" t="b">
         <v>1</v>
@@ -6583,7 +6583,7 @@
         <v>186</v>
       </c>
       <c r="C234" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D234" t="b">
         <v>1</v>
@@ -6609,7 +6609,7 @@
         <v>0</v>
       </c>
       <c r="E235" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F235" t="s">
         <v>6</v>
@@ -6669,7 +6669,7 @@
         <v>0</v>
       </c>
       <c r="E238" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F238" t="s">
         <v>6</v>
@@ -6709,7 +6709,7 @@
         <v>1</v>
       </c>
       <c r="E240" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F240" t="s">
         <v>6</v>
@@ -6743,13 +6743,13 @@
         <v>198</v>
       </c>
       <c r="C242" t="s">
+        <v>441</v>
+      </c>
+      <c r="D242" t="b">
+        <v>0</v>
+      </c>
+      <c r="E242" t="s">
         <v>442</v>
-      </c>
-      <c r="D242" t="b">
-        <v>0</v>
-      </c>
-      <c r="E242" t="s">
-        <v>443</v>
       </c>
       <c r="F242" t="s">
         <v>6</v>
@@ -6763,7 +6763,7 @@
         <v>198</v>
       </c>
       <c r="C243" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D243" t="b">
         <v>1</v>
@@ -6829,7 +6829,7 @@
         <v>0</v>
       </c>
       <c r="E246" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F246" t="s">
         <v>6</v>
@@ -6843,7 +6843,7 @@
         <v>200</v>
       </c>
       <c r="C247" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D247" t="b">
         <v>1</v>
@@ -6860,16 +6860,16 @@
         <v>247</v>
       </c>
       <c r="B248" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C248" t="s">
+        <v>446</v>
+      </c>
+      <c r="D248" t="b">
+        <v>1</v>
+      </c>
+      <c r="E248" t="s">
         <v>447</v>
-      </c>
-      <c r="D248" t="b">
-        <v>1</v>
-      </c>
-      <c r="E248" t="s">
-        <v>448</v>
       </c>
       <c r="F248" t="s">
         <v>6</v>
@@ -6880,16 +6880,16 @@
         <v>248</v>
       </c>
       <c r="B249" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C249" t="s">
+        <v>448</v>
+      </c>
+      <c r="D249" t="b">
+        <v>1</v>
+      </c>
+      <c r="E249" t="s">
         <v>449</v>
-      </c>
-      <c r="D249" t="b">
-        <v>1</v>
-      </c>
-      <c r="E249" t="s">
-        <v>450</v>
       </c>
       <c r="F249" t="s">
         <v>6</v>
@@ -6900,16 +6900,16 @@
         <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C250" t="s">
+        <v>450</v>
+      </c>
+      <c r="D250" t="b">
+        <v>0</v>
+      </c>
+      <c r="E250" t="s">
         <v>451</v>
-      </c>
-      <c r="D250" t="b">
-        <v>0</v>
-      </c>
-      <c r="E250" t="s">
-        <v>452</v>
       </c>
       <c r="F250" t="s">
         <v>6</v>
@@ -6920,7 +6920,7 @@
         <v>250</v>
       </c>
       <c r="B251" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C251" t="s">
         <v>203</v>
@@ -6929,7 +6929,7 @@
         <v>0</v>
       </c>
       <c r="E251" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F251" t="s">
         <v>6</v>
@@ -6940,7 +6940,7 @@
         <v>251</v>
       </c>
       <c r="B252" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C252" t="s">
         <v>204</v>
@@ -6949,7 +6949,7 @@
         <v>0</v>
       </c>
       <c r="E252" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F252" t="s">
         <v>6</v>
@@ -6960,7 +6960,7 @@
         <v>252</v>
       </c>
       <c r="B253" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C253" t="s">
         <v>205</v>
@@ -6969,7 +6969,7 @@
         <v>1</v>
       </c>
       <c r="E253" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F253" t="s">
         <v>6</v>
@@ -6980,7 +6980,7 @@
         <v>253</v>
       </c>
       <c r="B254" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C254" t="s">
         <v>206</v>
@@ -6989,7 +6989,7 @@
         <v>1</v>
       </c>
       <c r="E254" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F254" t="s">
         <v>6</v>
@@ -7000,7 +7000,7 @@
         <v>254</v>
       </c>
       <c r="B255" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C255" t="s">
         <v>207</v>
@@ -7009,7 +7009,7 @@
         <v>0</v>
       </c>
       <c r="E255" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F255" t="s">
         <v>6</v>
@@ -7020,7 +7020,7 @@
         <v>255</v>
       </c>
       <c r="B256" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C256" t="s">
         <v>208</v>
@@ -7029,7 +7029,7 @@
         <v>1</v>
       </c>
       <c r="E256" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F256" t="s">
         <v>6</v>
@@ -7063,7 +7063,7 @@
         <v>209</v>
       </c>
       <c r="C258" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D258" t="b">
         <v>1</v>
@@ -7129,7 +7129,7 @@
         <v>0</v>
       </c>
       <c r="E261" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F261" t="s">
         <v>6</v>
@@ -7143,7 +7143,7 @@
         <v>212</v>
       </c>
       <c r="C262" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D262" t="b">
         <v>1</v>
@@ -7160,7 +7160,7 @@
         <v>262</v>
       </c>
       <c r="B263" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C263" t="s">
         <v>215</v>
@@ -7169,7 +7169,7 @@
         <v>0</v>
       </c>
       <c r="E263" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F263" t="s">
         <v>6</v>
@@ -7180,16 +7180,16 @@
         <v>263</v>
       </c>
       <c r="B264" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C264" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D264" t="b">
         <v>1</v>
       </c>
       <c r="E264" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F264" t="s">
         <v>6</v>
@@ -7200,7 +7200,7 @@
         <v>264</v>
       </c>
       <c r="B265" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C265" t="s">
         <v>216</v>
@@ -7209,7 +7209,7 @@
         <v>0</v>
       </c>
       <c r="E265" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F265" t="s">
         <v>6</v>
@@ -7249,7 +7249,7 @@
         <v>0</v>
       </c>
       <c r="E267" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F267" t="s">
         <v>6</v>
@@ -7263,13 +7263,13 @@
         <v>220</v>
       </c>
       <c r="C268" t="s">
+        <v>464</v>
+      </c>
+      <c r="D268" t="b">
+        <v>0</v>
+      </c>
+      <c r="E268" t="s">
         <v>465</v>
-      </c>
-      <c r="D268" t="b">
-        <v>0</v>
-      </c>
-      <c r="E268" t="s">
-        <v>466</v>
       </c>
       <c r="F268" t="s">
         <v>6</v>
@@ -7289,7 +7289,7 @@
         <v>0</v>
       </c>
       <c r="E269" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F269" t="s">
         <v>6</v>
@@ -7323,13 +7323,13 @@
         <v>223</v>
       </c>
       <c r="C271" t="s">
+        <v>467</v>
+      </c>
+      <c r="D271" t="b">
+        <v>0</v>
+      </c>
+      <c r="E271" t="s">
         <v>468</v>
-      </c>
-      <c r="D271" t="b">
-        <v>0</v>
-      </c>
-      <c r="E271" t="s">
-        <v>469</v>
       </c>
       <c r="F271" t="s">
         <v>6</v>
@@ -7389,7 +7389,7 @@
         <v>0</v>
       </c>
       <c r="E274" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F274" t="s">
         <v>6</v>
@@ -7443,13 +7443,13 @@
         <v>230</v>
       </c>
       <c r="C277" t="s">
+        <v>470</v>
+      </c>
+      <c r="D277" t="b">
+        <v>1</v>
+      </c>
+      <c r="E277" t="s">
         <v>471</v>
-      </c>
-      <c r="D277" t="b">
-        <v>1</v>
-      </c>
-      <c r="E277" t="s">
-        <v>472</v>
       </c>
       <c r="F277" t="s">
         <v>6</v>
@@ -7469,7 +7469,7 @@
         <v>1</v>
       </c>
       <c r="E278" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F278" t="s">
         <v>6</v>
@@ -7483,13 +7483,13 @@
         <v>230</v>
       </c>
       <c r="C279" t="s">
+        <v>473</v>
+      </c>
+      <c r="D279" t="b">
+        <v>0</v>
+      </c>
+      <c r="E279" t="s">
         <v>474</v>
-      </c>
-      <c r="D279" t="b">
-        <v>0</v>
-      </c>
-      <c r="E279" t="s">
-        <v>475</v>
       </c>
       <c r="F279" t="s">
         <v>6</v>
@@ -7563,13 +7563,13 @@
         <v>236</v>
       </c>
       <c r="C283" t="s">
+        <v>475</v>
+      </c>
+      <c r="D283" t="b">
+        <v>0</v>
+      </c>
+      <c r="E283" t="s">
         <v>476</v>
-      </c>
-      <c r="D283" t="b">
-        <v>0</v>
-      </c>
-      <c r="E283" t="s">
-        <v>477</v>
       </c>
       <c r="F283" t="s">
         <v>6</v>
@@ -7583,13 +7583,13 @@
         <v>236</v>
       </c>
       <c r="C284" t="s">
+        <v>477</v>
+      </c>
+      <c r="D284" t="b">
+        <v>0</v>
+      </c>
+      <c r="E284" t="s">
         <v>478</v>
-      </c>
-      <c r="D284" t="b">
-        <v>0</v>
-      </c>
-      <c r="E284" t="s">
-        <v>479</v>
       </c>
       <c r="F284" t="s">
         <v>6</v>
@@ -7603,7 +7603,7 @@
         <v>236</v>
       </c>
       <c r="C285" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D285" t="b">
         <v>1</v>
@@ -7620,16 +7620,16 @@
         <v>285</v>
       </c>
       <c r="B286" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C286" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D286" t="b">
         <v>1</v>
       </c>
       <c r="E286" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F286" t="s">
         <v>6</v>
@@ -7640,7 +7640,7 @@
         <v>286</v>
       </c>
       <c r="B287" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C287" t="s">
         <v>237</v>
@@ -7649,7 +7649,7 @@
         <v>0</v>
       </c>
       <c r="E287" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F287" t="s">
         <v>6</v>
@@ -7660,16 +7660,16 @@
         <v>287</v>
       </c>
       <c r="B288" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C288" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D288" t="b">
         <v>1</v>
       </c>
       <c r="E288" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F288" t="s">
         <v>6</v>
@@ -7683,13 +7683,13 @@
         <v>238</v>
       </c>
       <c r="C289" t="s">
+        <v>482</v>
+      </c>
+      <c r="D289" t="b">
+        <v>0</v>
+      </c>
+      <c r="E289" t="s">
         <v>483</v>
-      </c>
-      <c r="D289" t="b">
-        <v>0</v>
-      </c>
-      <c r="E289" t="s">
-        <v>484</v>
       </c>
       <c r="F289" t="s">
         <v>6</v>
@@ -7763,13 +7763,13 @@
         <v>241</v>
       </c>
       <c r="C293" t="s">
+        <v>484</v>
+      </c>
+      <c r="D293" t="b">
+        <v>0</v>
+      </c>
+      <c r="E293" t="s">
         <v>485</v>
-      </c>
-      <c r="D293" t="b">
-        <v>0</v>
-      </c>
-      <c r="E293" t="s">
-        <v>486</v>
       </c>
       <c r="F293" t="s">
         <v>6</v>
@@ -7800,7 +7800,7 @@
         <v>294</v>
       </c>
       <c r="B295" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C295" t="s">
         <v>244</v>
@@ -7809,7 +7809,7 @@
         <v>0</v>
       </c>
       <c r="E295" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F295" t="s">
         <v>6</v>
@@ -7820,7 +7820,7 @@
         <v>295</v>
       </c>
       <c r="B296" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C296" t="s">
         <v>245</v>
@@ -7829,7 +7829,7 @@
         <v>1</v>
       </c>
       <c r="E296" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F296" t="s">
         <v>6</v>
@@ -7840,7 +7840,7 @@
         <v>296</v>
       </c>
       <c r="B297" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C297" t="s">
         <v>246</v>
@@ -7849,7 +7849,7 @@
         <v>1</v>
       </c>
       <c r="E297" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F297" t="s">
         <v>6</v>
@@ -7863,7 +7863,7 @@
         <v>247</v>
       </c>
       <c r="C298" t="s">
-        <v>248</v>
+        <v>495</v>
       </c>
       <c r="D298" t="b">
         <v>1</v>
@@ -7883,13 +7883,13 @@
         <v>247</v>
       </c>
       <c r="C299" t="s">
+        <v>486</v>
+      </c>
+      <c r="D299" t="b">
+        <v>0</v>
+      </c>
+      <c r="E299" t="s">
         <v>487</v>
-      </c>
-      <c r="D299" t="b">
-        <v>0</v>
-      </c>
-      <c r="E299" t="s">
-        <v>488</v>
       </c>
       <c r="F299" t="s">
         <v>6</v>
@@ -7903,13 +7903,13 @@
         <v>247</v>
       </c>
       <c r="C300" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D300" t="b">
         <v>0</v>
       </c>
       <c r="E300" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F300" t="s">
         <v>6</v>
@@ -7920,10 +7920,10 @@
         <v>300</v>
       </c>
       <c r="B301" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C301" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D301" t="b">
         <v>1</v>
@@ -7940,16 +7940,16 @@
         <v>301</v>
       </c>
       <c r="B302" t="s">
+        <v>249</v>
+      </c>
+      <c r="C302" t="s">
         <v>250</v>
       </c>
-      <c r="C302" t="s">
-        <v>251</v>
-      </c>
       <c r="D302" t="b">
         <v>0</v>
       </c>
       <c r="E302" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F302" t="s">
         <v>6</v>
@@ -7960,16 +7960,16 @@
         <v>302</v>
       </c>
       <c r="B303" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C303" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D303" t="b">
         <v>1</v>
       </c>
       <c r="E303" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F303" t="s">
         <v>6</v>
@@ -7980,10 +7980,10 @@
         <v>303</v>
       </c>
       <c r="B304" t="s">
+        <v>252</v>
+      </c>
+      <c r="C304" t="s">
         <v>253</v>
-      </c>
-      <c r="C304" t="s">
-        <v>254</v>
       </c>
       <c r="D304" t="b">
         <v>1</v>
@@ -8000,16 +8000,16 @@
         <v>304</v>
       </c>
       <c r="B305" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C305" t="s">
+        <v>492</v>
+      </c>
+      <c r="D305" t="b">
+        <v>0</v>
+      </c>
+      <c r="E305" t="s">
         <v>493</v>
-      </c>
-      <c r="D305" t="b">
-        <v>0</v>
-      </c>
-      <c r="E305" t="s">
-        <v>494</v>
       </c>
       <c r="F305" t="s">
         <v>6</v>
@@ -8020,10 +8020,10 @@
         <v>305</v>
       </c>
       <c r="B306" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C306" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D306" t="b">
         <v>1</v>
@@ -8040,10 +8040,10 @@
         <v>306</v>
       </c>
       <c r="B307" t="s">
+        <v>255</v>
+      </c>
+      <c r="C307" t="s">
         <v>256</v>
-      </c>
-      <c r="C307" t="s">
-        <v>257</v>
       </c>
       <c r="D307" t="b">
         <v>1</v>
@@ -8060,10 +8060,10 @@
         <v>307</v>
       </c>
       <c r="B308" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C308" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D308" t="b">
         <v>1</v>

</xml_diff>